<commit_message>
Additional features, templates, etc
</commit_message>
<xml_diff>
--- a/sw-config.xlsx
+++ b/sw-config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19155" windowHeight="6570"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19158" windowHeight="6570"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -75,12 +75,6 @@
     <t>First 6 characters of vendor mac address you want to match on</t>
   </si>
   <si>
-    <t>VendorVLAN</t>
-  </si>
-  <si>
-    <t>Vlan number of where these devices should be located</t>
-  </si>
-  <si>
     <t>LogLocation</t>
   </si>
   <si>
@@ -88,6 +82,12 @@
   </si>
   <si>
     <t>File Path for the Switchport Report</t>
+  </si>
+  <si>
+    <t>VendorTemplate</t>
+  </si>
+  <si>
+    <t>Template Name of where these devices should be sources (leave blank if none should be applied)</t>
   </si>
 </sst>
 </file>
@@ -428,17 +428,17 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="56.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.68359375" customWidth="1"/>
+    <col min="2" max="2" width="20.41796875" customWidth="1"/>
+    <col min="3" max="3" width="56.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -458,7 +458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -467,7 +467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -476,9 +476,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>13</v>
@@ -487,7 +487,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -495,20 +495,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -524,14 +524,14 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.26171875" customWidth="1"/>
+    <col min="2" max="2" width="16.15625" customWidth="1"/>
+    <col min="3" max="3" width="17.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>